<commit_message>
added another negative case
</commit_message>
<xml_diff>
--- a/TestCases_Register.xlsx
+++ b/TestCases_Register.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SoftUni\TeamProject\SRS-QA-Fundamentals\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="TestCase1" sheetId="1" r:id="rId1"/>
+    <sheet name="TestCase2" sheetId="2" r:id="rId2"/>
+    <sheet name="TestCase3" sheetId="3" r:id="rId3"/>
+    <sheet name="TestCase4" sheetId="4" r:id="rId4"/>
+    <sheet name="TestCase5" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="59">
   <si>
     <t>Team Antictra</t>
   </si>
@@ -164,12 +170,42 @@
   </si>
   <si>
     <t>The purpose of the test is to test if registration of a user with inccorrect input data is not allowed</t>
+  </si>
+  <si>
+    <t>Enter a username</t>
+  </si>
+  <si>
+    <t>Enter email</t>
+  </si>
+  <si>
+    <t>Enter valid email</t>
+  </si>
+  <si>
+    <t>pesho@pesho.com</t>
+  </si>
+  <si>
+    <t>A green tick should show, denoting that the mail is unique</t>
+  </si>
+  <si>
+    <t>Enter valid mail</t>
+  </si>
+  <si>
+    <t>gosho@gosho.com</t>
+  </si>
+  <si>
+    <t>A green tick should show, denoting that the email is unique</t>
+  </si>
+  <si>
+    <t>GoGO#67619</t>
+  </si>
+  <si>
+    <t>A red sign should be shown, along with a writing saying that the email is taken</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -208,12 +244,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -224,6 +264,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -272,7 +315,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -307,7 +350,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -516,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G17"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,15 +703,18 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
         <v>3</v>
       </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s">
-        <v>32</v>
+      <c r="B13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -676,13 +722,10 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
         <v>32</v>
-      </c>
-      <c r="D14" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -690,23 +733,38 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
         <v>34</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>38</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C11" r:id="rId1"/>
+    <hyperlink ref="C13" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -862,9 +920,9 @@
       <c r="A14" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -879,10 +937,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,11 +1014,11 @@
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1023,15 +1081,18 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
         <v>3</v>
       </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s">
-        <v>45</v>
+      <c r="B13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1039,13 +1100,10 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
         <v>45</v>
-      </c>
-      <c r="D14" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1053,29 +1111,44 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
         <v>34</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C11" r:id="rId1"/>
+    <hyperlink ref="C13" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1085,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,11 +1233,11 @@
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1231,9 +1304,9 @@
       <c r="A14" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1245,4 +1318,247 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="4" max="4" width="45.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>1</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>3</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B14:D14"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C11" r:id="rId1"/>
+    <hyperlink ref="C13" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>